<commit_message>
Atualização X e Y
</commit_message>
<xml_diff>
--- a/data/Producao_Bibliografica.xlsx
+++ b/data/Producao_Bibliografica.xlsx
@@ -8261,7 +8261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8358,6 +8358,386 @@
       <c r="C6" t="inlineStr">
         <is>
           <t>CASTANHO, G. Sad topics: an outline for the history of medieval sadness. BRATHAIR (ONLINE), 2023.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. Cais do Valongo: caminhos da África no Brasil. In: Silvana Terenzi Neuenschwander. (Org.). Patrimônios do Brasil. 1ed.Belo Horizonte: Lucca, 2022, v. , p. 156-165.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. Liberdade, liberdade, abre as asas sobre nós?. Revista Cult, p. 40 - 43, 01 set.  2022.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. História da África e dos Africanos no Brasil: patrimônios, história pública e reparação. 2021. (Apresentação de Trabalho/Conferência ou palestra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. Educação Patrimonial, História Pública e Reparação. 2021. (Apresentação de Trabalho/Conferência ou palestra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica; NASCIMENTO, Patricia ; OLIVEIRA, L. C. . Heranças Africanas no Brasil. 2021. (Apresentação de Trabalho/Conferência ou palestra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. Patrimônio afro-brasileiro e políticas públicas: uma questão de direitos. 2021. (Apresentação de Trabalho/Conferência ou palestra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. Trajetórias de africanas na luta por liberdade no Brasil. 2021. (Apresentação de Trabalho/Outra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. Escravidão e Liberdade: trajetórias africanas no Brasil. 2021. (Apresentação de Trabalho/Outra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. Passados sensíveis nos roteiros e aulas de campo na região do Cais do Valongo. 2021. (Apresentação de Trabalho/Outra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. Cosmovisão africana. 2021. (Apresentação de Trabalho/Conferência ou palestra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica; LIBERATO, Carlos Franco . Sylviane Diouf: quando os africanos resistem à escravidão. 2022. (Apresentação de Trabalho/Conferência ou palestra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica; NOGUERA, R. . Por uma Educação Antirracista. 2022. (Apresentação de Trabalho/Conferência ou palestra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. Educação paras as relações étnicorraciais e o Colégio de Aplicação da UFRJ. 2022. (Apresentação de Trabalho/Conferência ou palestra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. Histórias da escravidão e da liberdade na Pequena África carioca. 2023. (Apresentação de Trabalho/Conferência ou palestra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. Cais do Valongo: encruzilhada de histórias e memórias negras no Rio de Janeiro. 2023. (Apresentação de Trabalho/Conferência ou palestra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. O Cais do Valongo, a Pequena África e o Arquivo Nacional. 2023. (Apresentação de Trabalho/Outra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica; NOGUERA, R. . Por uma Educação Antirracista.
+						2021. (Desenvolvimento de material didático ou instrucional - CadernodeTextoseAtividades).</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica; BRAGA, Damião ; BRASIL, S. ; MOREIRA, G. M. . MPF assina acordo para valorização do memorial Cais do Valongo, no Rio de Janeiro. 2021.
+							(Programa de rádio ou TV/Entrevista).</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica; MUNDURUKU, Daniel . Heranças Africanas no Brasil. 2021.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica; MONTEIRO, Ana Maria da F Costa ; ROCHA, H. A. B. . Atividade de lançamento: Independência para quem? Espaços de reexistência. 2022.
+							(Programa de rádio ou TV/Outra).</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. A história da escravidão resiste aos apagamentos sucessivos na Pequena África carioca. 2022.
+							(Programa de rádio ou TV/Entrevista).</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica; SILVA JR, C. . Uma perspectiva negra sobre a independência do Brasil. 2022.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. Nossas Histórias n.48 - Rede de HistoriadorXs NegrXs. 2021.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. O Museu de História e Cultura Afro-brasileira e a história da população negra no Brasil. 2023.
+							(Programa de rádio ou TV/Entrevista).</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Mônica Lima e Souza</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>SOUZA, Mônica Lima e  OU  LIMA, Mônica OU LIMA, Monica. Vim de lá. 2023.</t>
         </is>
       </c>
     </row>

</xml_diff>